<commit_message>
precomiit to work w/chromebook
</commit_message>
<xml_diff>
--- a/Tracer Wire Request Form.xlsx
+++ b/Tracer Wire Request Form.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tabatha.Waugh\OneDrive - Rogers Communications Inc\2021\Damage Prevention Specialist\Tracer Wire Requests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{59C8F977-32BE-4533-9590-E471BD45A1F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F962C5A7-F6CD-48CF-966A-760713CD6FC0}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D06830BB-6C44-4073-86E0-30AC2E6ABEFB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -161,8 +155,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,17 +553,17 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C222C601-B709-4AFE-BF23-51204C884AB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C222C601-B709-4AFE-BF23-51204C884AB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -640,7 +634,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -692,7 +686,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -886,30 +880,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CAA614-AEA9-4940-BDE2-1187F23140C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1"/>
+    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -917,7 +911,7 @@
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -927,7 +921,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -937,7 +931,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -947,7 +941,7 @@
       </c>
       <c r="D6" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="18" customHeight="1" thickBot="1">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -957,7 +951,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="45.75" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -965,7 +959,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -973,7 +967,7 @@
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
     </row>
-    <row r="10" spans="1:4" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="51" customHeight="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>1</v>
       </c>
@@ -995,6 +989,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E09B0AB361BA4744B320CD0B6073471C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="889355d7fbab2a6f6232570d78685296">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9e9ea0fb-ef18-4e2b-9b7c-85d46f68bcfb" xmlns:ns4="05058eeb-84ec-4761-a2a4-4c7ab4af768e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9f6327b38a09322c4d3c40e13ba49d2" ns3:_="" ns4:_="">
     <xsd:import namespace="9e9ea0fb-ef18-4e2b-9b7c-85d46f68bcfb"/>
@@ -1217,22 +1226,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EDC68C4-FF0C-417D-9BDD-1754D55621B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{719AA484-782D-4FF0-90E2-3772CE61B0F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0441160-B6CE-46C7-B5E0-9964FD82E0F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1249,21 +1260,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{719AA484-782D-4FF0-90E2-3772CE61B0F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EDC68C4-FF0C-417D-9BDD-1754D55621B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>